<commit_message>
Cambio menu mobile + otros Jul 2024
</commit_message>
<xml_diff>
--- a/Cobros.xlsx
+++ b/Cobros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Santiago\python\Ecommerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFE063D-42CC-476A-8601-F38EEE4B371F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661892A2-2138-4F98-93F0-2050CECE7559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{25B8D9A2-7021-4189-AD08-0DB7E4AC3B63}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{25B8D9A2-7021-4189-AD08-0DB7E4AC3B63}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={62BBC310-C1ED-4398-89F7-821B37461F24}</author>
+  </authors>
+  <commentList>
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{62BBC310-C1ED-4398-89F7-821B37461F24}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Valor real USD 1280</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>Transferencia Mariano</t>
   </si>
@@ -66,18 +84,31 @@
   </si>
   <si>
     <t>Milena Sofia Morales</t>
+  </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abono Anual 2024 </t>
+  </si>
+  <si>
+    <t>Silvia Barros Reyes</t>
+  </si>
+  <si>
+    <t>Extra x Dif pago Tarjeta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-[$USD]\ * #,##0.00_-;\-[$USD]\ * #,##0.00_-;_-[$USD]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,8 +131,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,6 +148,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,20 +244,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -231,6 +279,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="De Bony, Santiago Jorge" id="{2D481269-5F10-479C-91C9-085A47955C0A}" userId="S::santiago.debony@cencosud.com.ar::9ba76e4f-f517-4f9e-bf8a-0c21af19553c" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -548,142 +602,193 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G6" dT="2024-06-14T19:00:12.04" personId="{2D481269-5F10-479C-91C9-085A47955C0A}" id="{62BBC310-C1ED-4398-89F7-821B37461F24}">
+    <text>Valor real USD 1280</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B90A81-C9CF-47E5-94B3-7AE5358343FA}">
-  <dimension ref="B2:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B90A81-C9CF-47E5-94B3-7AE5358343FA}">
+  <dimension ref="B2:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="12">
         <v>45376</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="14">
         <v>58250</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="14">
         <v>1010</v>
       </c>
-      <c r="G3" s="5">
-        <f>+E3/F3</f>
+      <c r="H3" s="15">
+        <f>+F3/G3</f>
         <v>57.67326732673267</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="12">
         <v>45377</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="14">
         <v>11877</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="14">
         <v>1005</v>
       </c>
-      <c r="G4" s="5">
-        <f>+E4/F4</f>
+      <c r="H4" s="15">
+        <f>+F4/G4</f>
         <v>11.817910447761195</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
         <v>45377</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="14">
         <v>14165</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="14">
         <v>1005</v>
       </c>
-      <c r="G5" s="5">
-        <f>+E5/F5</f>
+      <c r="H5" s="15">
+        <f>+F5/G5</f>
         <v>14.09452736318408</v>
       </c>
+      <c r="J5" s="11"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="5"/>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="12">
+        <v>45457</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="14">
+        <v>33000</v>
+      </c>
+      <c r="G6" s="14">
+        <v>2010.44</v>
+      </c>
+      <c r="H6" s="15">
+        <f>+F6/G6</f>
+        <v>16.414317263882534</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="5"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4"/>
+      <c r="J7" s="11"/>
     </row>
-    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
     </row>
-    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="8">
-        <f>SUM(E3:E8)</f>
-        <v>84292</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10">
-        <f>SUM(G3:G8)</f>
-        <v>83.585705137677948</v>
-      </c>
+    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="7">
+        <f>SUM(F3:F8)</f>
+        <v>117292</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9">
+        <f>SUM(H3:H8)</f>
+        <v>100.00002240156049</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>